<commit_message>
add New company page
</commit_message>
<xml_diff>
--- a/testData/FreeCrmTestData.xlsx
+++ b/testData/FreeCrmTestData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiva\OneDrive\Desktop\Shiva's Workspace\FreeCRMTest\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F44026-1B55-42AF-BDCD-03E5C5FC56C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F42570-DEB0-40C8-94EE-A0122886A697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{B0832FAE-82D6-44CA-A229-9EA1CEF89E98}"/>
+    <workbookView xWindow="1500" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{B0832FAE-82D6-44CA-A229-9EA1CEF89E98}"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
+    <sheet name="companies" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>title</t>
   </si>
@@ -72,6 +73,42 @@
   </si>
   <si>
     <t>Bebo</t>
+  </si>
+  <si>
+    <t>industry</t>
+  </si>
+  <si>
+    <t>numberofemploye</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Event</t>
   </si>
 </sst>
 </file>
@@ -87,7 +124,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -97,6 +134,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -113,9 +156,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,7 +476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A859595-BD06-43CD-8948-BD2CB15B1CBC}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
@@ -500,4 +544,74 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0907EDFC-4997-4E01-9DBE-3F3993A55BF9}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <v>10005</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3">
+        <v>5263</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>